<commit_message>
TestNG XML + Data Sheet
</commit_message>
<xml_diff>
--- a/data/TC002.xlsx
+++ b/data/TC002.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>UserName</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>LeafTaps</t>
-  </si>
-  <si>
-    <t>LeafTaps123</t>
   </si>
   <si>
     <t>Manager</t>
@@ -461,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -510,7 +507,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
@@ -525,39 +522,12 @@
         <v>11</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>